<commit_message>
add script for work profile user
</commit_message>
<xml_diff>
--- a/list.xlsx
+++ b/list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11550"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11550" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="list7" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2390" uniqueCount="1091">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2526" uniqueCount="1093">
   <si>
     <t>ChnTelecomAutoReg.apk</t>
   </si>
@@ -3464,6 +3464,14 @@
   </si>
   <si>
     <t>路径</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>pm hide --user 11</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>pm uninstall --user 11</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -4144,7 +4152,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4188,6 +4196,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -4514,7 +4525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H189"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8286,7 +8297,7 @@
   <dimension ref="A1:H195"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -13070,287 +13081,699 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.5" style="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.375" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>1089</v>
       </c>
       <c r="B1" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D1" t="s">
+        <v>257</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="F1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>1089</v>
       </c>
       <c r="B2" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="F2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>1089</v>
       </c>
       <c r="B3" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D3" t="s">
+        <v>273</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="F3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>1089</v>
       </c>
       <c r="B4" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D4" t="s">
+        <v>284</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="F4" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>1089</v>
       </c>
       <c r="B5" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D5" t="s">
+        <v>233</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="F5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>1089</v>
       </c>
       <c r="B6" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D6" t="s">
+        <v>239</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="F6" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>1089</v>
       </c>
       <c r="B7" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D7" t="s">
+        <v>354</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="F7" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>1089</v>
       </c>
       <c r="B8" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="F8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>1089</v>
       </c>
       <c r="B9" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="F9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>1089</v>
       </c>
       <c r="B10" t="s">
         <v>966</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D10" t="s">
+        <v>966</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="F10" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
         <v>1089</v>
       </c>
       <c r="B11" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D11" t="s">
+        <v>294</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="F11" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
         <v>1089</v>
       </c>
       <c r="B12" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D12" t="s">
+        <v>146</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="F12" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
         <v>1089</v>
       </c>
       <c r="B13" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D13" t="s">
+        <v>292</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="F13" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
         <v>1089</v>
       </c>
       <c r="B14" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D14" t="s">
+        <v>296</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="F14" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
         <v>1089</v>
       </c>
       <c r="B15" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D15" t="s">
+        <v>84</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="F15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
         <v>1089</v>
       </c>
       <c r="B16" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="F16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
         <v>1089</v>
       </c>
       <c r="B17" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="F17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
         <v>1089</v>
       </c>
       <c r="B18" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="F18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
         <v>1089</v>
       </c>
       <c r="B19" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D19" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="F19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
         <v>1089</v>
       </c>
       <c r="B20" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D20" t="s">
+        <v>961</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>1092</v>
+      </c>
+      <c r="F20" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
         <v>1089</v>
       </c>
       <c r="B21" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D21" t="s">
+        <v>305</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>1092</v>
+      </c>
+      <c r="F21" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
         <v>1089</v>
       </c>
       <c r="B22" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D22" t="s">
+        <v>161</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>1092</v>
+      </c>
+      <c r="F22" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
         <v>1089</v>
       </c>
       <c r="B23" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D23" t="s">
+        <v>176</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>1092</v>
+      </c>
+      <c r="F23" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="13" t="s">
         <v>1089</v>
       </c>
       <c r="B24" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D24" t="s">
+        <v>169</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>1092</v>
+      </c>
+      <c r="F24" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="13" t="s">
         <v>1089</v>
       </c>
       <c r="B25" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D25" t="s">
+        <v>120</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>1092</v>
+      </c>
+      <c r="F25" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="13" t="s">
         <v>1089</v>
       </c>
       <c r="B26" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C26" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D26" t="s">
+        <v>118</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>1092</v>
+      </c>
+      <c r="F26" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="13" t="s">
         <v>1089</v>
       </c>
       <c r="B27" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C27" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D27" t="s">
+        <v>173</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>1092</v>
+      </c>
+      <c r="F27" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="13" t="s">
         <v>1089</v>
       </c>
       <c r="B28" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C28" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D28" t="s">
+        <v>217</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>1092</v>
+      </c>
+      <c r="F28" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="13" t="s">
         <v>1089</v>
       </c>
       <c r="B29" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D29" t="s">
+        <v>175</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>1092</v>
+      </c>
+      <c r="F29" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="13" t="s">
         <v>1089</v>
       </c>
       <c r="B30" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C30" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D30" t="s">
+        <v>180</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>1092</v>
+      </c>
+      <c r="F30" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="13" t="s">
         <v>1089</v>
       </c>
       <c r="B31" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C31" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D31" t="s">
+        <v>92</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>1092</v>
+      </c>
+      <c r="F31" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="13" t="s">
         <v>1089</v>
       </c>
       <c r="B32" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D32" t="s">
+        <v>183</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>1092</v>
+      </c>
+      <c r="F32" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="13" t="s">
         <v>1089</v>
       </c>
       <c r="B33" t="s">
         <v>1010</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1010</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>1092</v>
+      </c>
+      <c r="F33" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="13" t="s">
         <v>1089</v>
       </c>
       <c r="B34" t="s">
+        <v>213</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D34" t="s">
+        <v>213</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>1092</v>
+      </c>
+      <c r="F34" t="s">
         <v>213</v>
       </c>
     </row>

</xml_diff>